<commit_message>
Worked: seperate A11 and before removing codes for full A11
</commit_message>
<xml_diff>
--- a/working/Perturb/notebooks/MatrixA11.xlsx
+++ b/working/Perturb/notebooks/MatrixA11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab_codes\FEM\FiniteElemntMethod\working\Perturb\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA2C5B5-6E53-4BB6-A87B-A6F05DE6D929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27592F7-16DE-45E3-8CB1-897A21D2765F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23964" yWindow="1608" windowWidth="16440" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23508" yWindow="1380" windowWidth="16440" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>